<commit_message>
Correctly increment index when encountering empty rows
</commit_message>
<xml_diff>
--- a/tests/Example 1.xlsx
+++ b/tests/Example 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayoub/Documents/goaluin/data-duplication-solution/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0857824-C3C2-6E4F-890B-8CA40FD1B20C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015E3DC3-8EA7-044E-B953-997BF8C2A6E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24260" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
   <si>
     <t xml:space="preserve">Nom et Prénom </t>
   </si>
@@ -167,15 +167,6 @@
     <t>Person 6</t>
   </si>
   <si>
-    <t>kd12327</t>
-  </si>
-  <si>
-    <t>Person 7</t>
-  </si>
-  <si>
-    <t>kd12328</t>
-  </si>
-  <si>
     <t>Person 8</t>
   </si>
   <si>
@@ -210,9 +201,6 @@
   </si>
   <si>
     <t>person6@gmail.com</t>
-  </si>
-  <si>
-    <t>person7@gmail.com</t>
   </si>
   <si>
     <t>person8@gmail.com</t>
@@ -554,11 +542,14 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -581,9 +572,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -805,7 +793,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -838,47 +826,47 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="24" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="23"/>
     </row>
     <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -888,37 +876,37 @@
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="23"/>
       <c r="L2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="N2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="27" t="s">
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="22"/>
-      <c r="X2" s="28">
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="29">
         <v>45385</v>
       </c>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="22"/>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="23"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
@@ -1081,7 +1069,7 @@
         <v>87123039214</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>32</v>
@@ -1119,14 +1107,14 @@
         <v>14</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
@@ -1159,7 +1147,7 @@
         <v>87123039215</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>32</v>
@@ -1203,7 +1191,7 @@
         <v>87123039216</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>32</v>
@@ -1247,10 +1235,10 @@
         <v>87123039217</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F10" s="15">
         <v>45327</v>
@@ -1291,17 +1279,13 @@
         <v>87123039218</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="15">
-        <v>45328</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>48</v>
-      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
@@ -1323,27 +1307,13 @@
       <c r="Z11" s="12"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11">
-        <v>8</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="9">
-        <v>87123039219</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="15">
-        <v>45329</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>50</v>
-      </c>
+      <c r="A12" s="11"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
@@ -1353,9 +1323,7 @@
       <c r="N12" s="12"/>
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
-      <c r="Q12" s="12" t="s">
-        <v>33</v>
-      </c>
+      <c r="Q12" s="12"/>
       <c r="R12" s="12"/>
       <c r="S12" s="12"/>
       <c r="T12" s="12"/>
@@ -1371,13 +1339,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C13" s="9">
         <v>87123039220</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>32</v>
@@ -1386,7 +1354,7 @@
         <v>45330</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10" t="s">
@@ -1415,13 +1383,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C14" s="9">
         <v>87123039221</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>32</v>
@@ -1430,7 +1398,7 @@
         <v>45331</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
@@ -1459,13 +1427,13 @@
         <v>11</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C15" s="9">
         <v>87123039222</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>32</v>
@@ -1474,7 +1442,7 @@
         <v>45332</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
@@ -1503,22 +1471,22 @@
         <v>12</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C16" s="9">
         <v>87123039217</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F16" s="15">
         <v>38022</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
@@ -20668,11 +20636,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="H2:K2"/>
@@ -20681,6 +20644,11 @@
     <mergeCell ref="N2:S2"/>
     <mergeCell ref="T2:W2"/>
     <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
@@ -20693,15 +20661,14 @@
     <hyperlink ref="D5" r:id="rId2" xr:uid="{6626B44E-5A2F-D240-8CF5-A5B7EBED9E87}"/>
     <hyperlink ref="D6" r:id="rId3" xr:uid="{2C47EE9B-1387-CA41-B24C-1ECC140D05C0}"/>
     <hyperlink ref="D11" r:id="rId4" xr:uid="{669BEEFF-5649-CB48-8E3B-83D4963693E9}"/>
-    <hyperlink ref="D12" r:id="rId5" xr:uid="{44CB9E20-50D4-8644-A295-C5EBB01882BB}"/>
-    <hyperlink ref="D13" r:id="rId6" xr:uid="{15B6C303-DF2B-6646-904B-D627463D7F95}"/>
-    <hyperlink ref="D14" r:id="rId7" xr:uid="{A7A7BB63-2591-5E40-B267-E1DB84DFCAB8}"/>
-    <hyperlink ref="D15" r:id="rId8" xr:uid="{DBCC3DD6-5271-5B49-BD1F-0AB4A54B0EDF}"/>
-    <hyperlink ref="D9" r:id="rId9" xr:uid="{5716625C-FDE7-3E46-897F-2CCED3205B41}"/>
-    <hyperlink ref="D10" r:id="rId10" xr:uid="{3456F1E6-674B-D44B-8030-F52EE3DFD59B}"/>
-    <hyperlink ref="D16" r:id="rId11" xr:uid="{2E4FA2D7-472D-A347-9540-08EE7D917D12}"/>
-    <hyperlink ref="D17" r:id="rId12" xr:uid="{91C50B2C-FBBD-B34A-8F6E-CE5CE7C25692}"/>
-    <hyperlink ref="D8" r:id="rId13" xr:uid="{A73B760C-49FD-9148-BB43-3C1261A4DF17}"/>
+    <hyperlink ref="D13" r:id="rId5" xr:uid="{15B6C303-DF2B-6646-904B-D627463D7F95}"/>
+    <hyperlink ref="D14" r:id="rId6" xr:uid="{A7A7BB63-2591-5E40-B267-E1DB84DFCAB8}"/>
+    <hyperlink ref="D15" r:id="rId7" xr:uid="{DBCC3DD6-5271-5B49-BD1F-0AB4A54B0EDF}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{5716625C-FDE7-3E46-897F-2CCED3205B41}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{3456F1E6-674B-D44B-8030-F52EE3DFD59B}"/>
+    <hyperlink ref="D16" r:id="rId10" xr:uid="{2E4FA2D7-472D-A347-9540-08EE7D917D12}"/>
+    <hyperlink ref="D17" r:id="rId11" xr:uid="{91C50B2C-FBBD-B34A-8F6E-CE5CE7C25692}"/>
+    <hyperlink ref="D8" r:id="rId12" xr:uid="{A73B760C-49FD-9148-BB43-3C1261A4DF17}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>